<commit_message>
Adjusted costs for reference years 2025, 2030, 2040 and 2050 + added seperate technology catalogue for HC, MeOH and NH3
</commit_message>
<xml_diff>
--- a/input_data/extra_data/extra_data_processes.xlsx
+++ b/input_data/extra_data/extra_data_processes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vitoresearch-my.sharepoint.com/personal/hans_vandeput_vito_be/Documents/Mopo/mopo_repo/input_data/extra_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{EE620E29-61A6-43EA-BFBF-83AA0D58C3C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D81E28B4-8AED-430E-8704-76E8AE7E2675}"/>
+  <xr:revisionPtr revIDLastSave="139" documentId="8_{EE620E29-61A6-43EA-BFBF-83AA0D58C3C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{244FB31C-DAFE-48FB-81FB-B742A6F8C873}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{F2053A1D-A610-4EC9-BADA-756186C5C9C1}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="67">
   <si>
     <t>CO2</t>
   </si>
@@ -193,13 +193,58 @@
   </si>
   <si>
     <t>(eur-yr)/mwh</t>
+  </si>
+  <si>
+    <t>Remark</t>
+  </si>
+  <si>
+    <t>value of 2025 is average of 2020 and 2030</t>
+  </si>
+  <si>
+    <t>value of 2025 is average of 2020 and 2031</t>
+  </si>
+  <si>
+    <t>value of 2025 is average of 2020 and 2032</t>
+  </si>
+  <si>
+    <t>value of 2025 is average of 2020 and 2033</t>
+  </si>
+  <si>
+    <t>value of 2025 is average of 2020 and 2034</t>
+  </si>
+  <si>
+    <t>value of 2025 is average of 2020 and 2035</t>
+  </si>
+  <si>
+    <t>value of 2025 is average of 2020 and 2036</t>
+  </si>
+  <si>
+    <t>value of 2025 is average of 2020 and 2037</t>
+  </si>
+  <si>
+    <t>value of 2025 is average of 2020 and 2038</t>
+  </si>
+  <si>
+    <t>value of 2025 is average of 2020 and 2039</t>
+  </si>
+  <si>
+    <t>eur-yr/mwh</t>
+  </si>
+  <si>
+    <t>meur-yr/pj</t>
+  </si>
+  <si>
+    <t>meur/gw</t>
+  </si>
+  <si>
+    <t>meur-yr/gwh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,8 +260,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -226,6 +277,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -242,14 +299,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -268,9 +327,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -308,7 +367,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -414,7 +473,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -556,7 +615,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -564,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41472E5A-EAB6-4D4D-BEEA-89BED4F25E24}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18:I20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" activeCellId="1" sqref="B2 B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -580,7 +639,7 @@
     <col min="7" max="7" width="25.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -599,17 +658,23 @@
       <c r="F1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="G1" s="6">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="6">
+        <v>2025</v>
+      </c>
+      <c r="I1" s="6">
+        <v>2030</v>
+      </c>
+      <c r="J1" s="6">
+        <v>2040</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -626,16 +691,22 @@
         <v>1</v>
       </c>
       <c r="G2">
+        <v>270.51532941943901</v>
+      </c>
+      <c r="H2">
+        <v>238.23036063740565</v>
+      </c>
+      <c r="I2">
         <v>205.94539185537229</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>141.73888733575623</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>116.29857422421023</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -652,16 +723,22 @@
         <v>2</v>
       </c>
       <c r="G3">
+        <v>17.97</v>
+      </c>
+      <c r="H3">
+        <v>15.734999999999999</v>
+      </c>
+      <c r="I3">
         <v>13.5</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>9.0399999999999991</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>7.87</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -686,8 +763,14 @@
       <c r="I4">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J4">
+        <v>25</v>
+      </c>
+      <c r="K4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -707,16 +790,22 @@
         <v>34</v>
       </c>
       <c r="G5">
+        <v>7.1428571428571435E-3</v>
+      </c>
+      <c r="H5">
+        <v>7.1428571428571435E-3</v>
+      </c>
+      <c r="I5">
         <v>1.4285714285714287E-2</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>1.3698630136986302E-2</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>1.3333333333333334E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -736,16 +825,22 @@
         <v>34</v>
       </c>
       <c r="G6">
+        <v>1.4214285714285715</v>
+      </c>
+      <c r="H6">
+        <v>1.4214285714285715</v>
+      </c>
+      <c r="I6">
         <v>1.4285714285714286</v>
       </c>
-      <c r="H6">
+      <c r="J6">
         <v>1.3698630136986301</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <v>1.3333333333333333</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -765,16 +860,22 @@
         <v>34</v>
       </c>
       <c r="G7">
+        <v>0.34789644012944981</v>
+      </c>
+      <c r="H7">
+        <v>0.33171521035598706</v>
+      </c>
+      <c r="I7">
         <v>0.3155339805825243</v>
       </c>
-      <c r="H7">
+      <c r="J7">
         <v>0.29126213592233013</v>
       </c>
-      <c r="I7">
+      <c r="K7">
         <v>0.26699029126213591</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -799,8 +900,14 @@
       <c r="I8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -825,8 +932,14 @@
       <c r="I9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -843,16 +956,22 @@
         <v>1</v>
       </c>
       <c r="G10">
+        <v>163.54487000279565</v>
+      </c>
+      <c r="H10">
+        <v>163.54487000279565</v>
+      </c>
+      <c r="I10">
         <v>132.04733948373871</v>
       </c>
-      <c r="H10">
+      <c r="J10">
         <v>116.29857422421023</v>
       </c>
-      <c r="I10">
+      <c r="K10">
         <v>105.39558289069052</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -869,16 +988,22 @@
         <v>2</v>
       </c>
       <c r="G11">
+        <v>4.7246295778585408</v>
+      </c>
+      <c r="H11">
+        <v>4.7246295778585408</v>
+      </c>
+      <c r="I11">
         <v>3.6343304445065696</v>
       </c>
-      <c r="H11">
+      <c r="J11">
         <v>3.6343304445065696</v>
       </c>
-      <c r="I11">
+      <c r="K11">
         <v>3.1497530519056935</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -903,8 +1028,14 @@
       <c r="I12">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J12">
+        <v>30</v>
+      </c>
+      <c r="K12">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -932,8 +1063,14 @@
       <c r="I13">
         <v>1.8083182640144666E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J13">
+        <v>1.8083182640144666E-2</v>
+      </c>
+      <c r="K13">
+        <v>1.8083182640144666E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -961,8 +1098,14 @@
       <c r="I14">
         <v>1.1573236889692586</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J14">
+        <v>1.1573236889692586</v>
+      </c>
+      <c r="K14">
+        <v>1.1573236889692586</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -990,8 +1133,14 @@
       <c r="I15">
         <v>0.25316455696202528</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J15">
+        <v>0.25316455696202528</v>
+      </c>
+      <c r="K15">
+        <v>0.25316455696202528</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1016,8 +1165,14 @@
       <c r="I16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1042,8 +1197,14 @@
       <c r="I17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -1071,8 +1232,14 @@
       <c r="I18">
         <v>7.3145990404386581</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J18">
+        <v>7.3145990404386581</v>
+      </c>
+      <c r="K18">
+        <v>7.3145990404386581</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -1100,8 +1267,14 @@
       <c r="I19">
         <v>0.3652392947103274</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J19">
+        <v>0.3652392947103274</v>
+      </c>
+      <c r="K19">
+        <v>0.3652392947103274</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -1127,6 +1300,12 @@
         <v>0.57934508816120911</v>
       </c>
       <c r="I20">
+        <v>0.57934508816120911</v>
+      </c>
+      <c r="J20">
+        <v>0.57934508816120911</v>
+      </c>
+      <c r="K20">
         <v>0.57934508816120911</v>
       </c>
     </row>
@@ -1137,10 +1316,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3BBEA03-D463-44FB-8E40-6A1CC8E39C5E}">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1150,13 +1329,14 @@
     <col min="3" max="3" width="14.44140625" customWidth="1"/>
     <col min="4" max="4" width="23.88671875" customWidth="1"/>
     <col min="5" max="5" width="29.88671875" customWidth="1"/>
-    <col min="6" max="7" width="14.44140625" customWidth="1"/>
-    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.21875" customWidth="1"/>
-    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="6" max="8" width="14.44140625" customWidth="1"/>
+    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.21875" customWidth="1"/>
+    <col min="11" max="11" width="15" customWidth="1"/>
+    <col min="12" max="12" width="35.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1175,17 +1355,26 @@
       <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="4">
+        <v>2025</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -1202,19 +1391,30 @@
         <v>1</v>
       </c>
       <c r="G2" s="3">
-        <f>G4*1000000/(365*24*(49/52))</f>
+        <f t="shared" ref="G2:K2" si="0">G4*1000000/(365*24*(49/52))</f>
+        <v>270.51532941943901</v>
+      </c>
+      <c r="H2" s="3">
+        <f t="shared" ref="H2" si="1">H4*1000000/(365*24*(49/52))</f>
+        <v>238.23036063740565</v>
+      </c>
+      <c r="I2" s="3">
+        <f>I4*1000000/(365*24*(49/52))</f>
         <v>205.94539185537229</v>
       </c>
-      <c r="H2" s="3">
-        <f t="shared" ref="H2:I2" si="0">H4*1000000/(365*24*(49/52))</f>
+      <c r="J2" s="3">
+        <f t="shared" si="0"/>
         <v>141.73888733575623</v>
       </c>
-      <c r="I2" s="3">
+      <c r="K2" s="3">
         <f t="shared" si="0"/>
         <v>116.29857422421023</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L2" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -1231,23 +1431,34 @@
         <v>2</v>
       </c>
       <c r="G3" s="3">
-        <f>G5</f>
+        <f t="shared" ref="G3:K3" si="2">G5</f>
+        <v>17.97</v>
+      </c>
+      <c r="H3" s="3">
+        <f t="shared" ref="H3" si="3">H5</f>
+        <v>15.734999999999999</v>
+      </c>
+      <c r="I3" s="3">
+        <f>I5</f>
         <v>13.5</v>
       </c>
-      <c r="H3" s="3">
-        <f t="shared" ref="H3:I3" si="1">H5</f>
+      <c r="J3" s="3">
+        <f t="shared" si="2"/>
         <v>9.0399999999999991</v>
       </c>
-      <c r="I3" s="3">
-        <f t="shared" si="1"/>
+      <c r="K3" s="3">
+        <f t="shared" si="2"/>
         <v>7.87</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L3" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s">
         <v>40</v>
       </c>
       <c r="D4" t="s">
@@ -1260,20 +1471,30 @@
         <v>1</v>
       </c>
       <c r="G4">
+        <v>2.2330000000000001</v>
+      </c>
+      <c r="H4" s="5">
+        <f>AVERAGE((G4,I4))</f>
+        <v>1.9664999999999999</v>
+      </c>
+      <c r="I4">
         <v>1.7</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>1.17</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>0.96</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L4" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s">
         <v>40</v>
       </c>
       <c r="D5" t="s">
@@ -1286,16 +1507,26 @@
         <v>2</v>
       </c>
       <c r="G5">
+        <v>17.97</v>
+      </c>
+      <c r="H5" s="5">
+        <f>AVERAGE((G5,I5))</f>
+        <v>15.734999999999999</v>
+      </c>
+      <c r="I5">
         <v>13.5</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>9.0399999999999991</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>7.87</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L5" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -1315,13 +1546,23 @@
         <v>25</v>
       </c>
       <c r="H6" s="3">
+        <f>AVERAGE((G6,I6))</f>
         <v>25</v>
       </c>
       <c r="I6" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J6" s="3">
+        <v>25</v>
+      </c>
+      <c r="K6" s="3">
+        <v>25</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -1341,19 +1582,30 @@
         <v>34</v>
       </c>
       <c r="G7" s="3">
-        <f>0.01/0.7</f>
-        <v>1.4285714285714287E-2</v>
+        <f>0.005/0.7</f>
+        <v>7.1428571428571435E-3</v>
       </c>
       <c r="H7" s="3">
-        <f>0.01/0.73</f>
-        <v>1.3698630136986302E-2</v>
+        <f>AVERAGE((G7,I7))</f>
+        <v>7.1428571428571435E-3</v>
       </c>
       <c r="I7" s="3">
-        <f>0.01/0.75</f>
-        <v>1.3333333333333334E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f>0.005/0.7</f>
+        <v>7.1428571428571435E-3</v>
+      </c>
+      <c r="J7" s="3">
+        <f t="shared" ref="J7:K7" si="4">0.005/0.7</f>
+        <v>7.1428571428571435E-3</v>
+      </c>
+      <c r="K7" s="3">
+        <f t="shared" si="4"/>
+        <v>7.1428571428571435E-3</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -1373,19 +1625,30 @@
         <v>34</v>
       </c>
       <c r="G8" s="3">
-        <f>1/0.7</f>
-        <v>1.4285714285714286</v>
+        <f>0.995/0.7</f>
+        <v>1.4214285714285715</v>
       </c>
       <c r="H8" s="3">
-        <f>1/0.73</f>
-        <v>1.3698630136986301</v>
+        <f>AVERAGE((G8,I8))</f>
+        <v>1.4214285714285715</v>
       </c>
       <c r="I8" s="3">
-        <f>1/0.75</f>
-        <v>1.3333333333333333</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" ref="I8:K8" si="5">0.995/0.7</f>
+        <v>1.4214285714285715</v>
+      </c>
+      <c r="J8" s="3">
+        <f t="shared" si="5"/>
+        <v>1.4214285714285715</v>
+      </c>
+      <c r="K8" s="3">
+        <f t="shared" si="5"/>
+        <v>1.4214285714285715</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
@@ -1405,19 +1668,30 @@
         <v>34</v>
       </c>
       <c r="G9" s="3">
-        <f>3.9/$I$41</f>
+        <f>4.3/$J$41</f>
+        <v>0.34789644012944981</v>
+      </c>
+      <c r="H9" s="3">
+        <f>AVERAGE((G9,I9))</f>
+        <v>0.33171521035598706</v>
+      </c>
+      <c r="I9" s="3">
+        <f>3.9/$J$41</f>
         <v>0.3155339805825243</v>
       </c>
-      <c r="H9" s="3">
-        <f>3.6/$I$41</f>
+      <c r="J9" s="3">
+        <f>3.6/$J$41</f>
         <v>0.29126213592233013</v>
       </c>
-      <c r="I9" s="3">
-        <f>3.3/$I$41</f>
+      <c r="K9" s="3">
+        <f>3.3/$J$41</f>
         <v>0.26699029126213591</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L9" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -1437,13 +1711,23 @@
         <v>0</v>
       </c>
       <c r="H10" s="3">
+        <f>AVERAGE((G10,I10))</f>
         <v>0</v>
       </c>
       <c r="I10" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J10" s="3">
+        <v>0</v>
+      </c>
+      <c r="K10" s="3">
+        <v>0</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
@@ -1463,13 +1747,23 @@
         <v>0</v>
       </c>
       <c r="H11" s="3">
+        <f>AVERAGE((G11,I11))</f>
         <v>0</v>
       </c>
       <c r="I11" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" s="3" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J11" s="3">
+        <v>0</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="3" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -1486,19 +1780,27 @@
         <v>1</v>
       </c>
       <c r="G13" s="3">
-        <f>G15*1000000/(365*24*(49/52))</f>
+        <f t="shared" ref="G13:H13" si="6">G15*1000000/(365*24*(49/52))</f>
+        <v>163.54487000279565</v>
+      </c>
+      <c r="H13" s="3">
+        <f t="shared" si="6"/>
+        <v>163.54487000279565</v>
+      </c>
+      <c r="I13" s="3">
+        <f>I15*1000000/(365*24*(49/52))</f>
         <v>132.04733948373871</v>
       </c>
-      <c r="H13" s="3">
-        <f t="shared" ref="H13:I13" si="2">H15*1000000/(365*24*(49/52))</f>
+      <c r="J13" s="3">
+        <f t="shared" ref="J13:K13" si="7">J15*1000000/(365*24*(49/52))</f>
         <v>116.29857422421023</v>
       </c>
-      <c r="I13" s="3">
-        <f t="shared" si="2"/>
+      <c r="K13" s="3">
+        <f t="shared" si="7"/>
         <v>105.39558289069052</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
@@ -1515,19 +1817,27 @@
         <v>2</v>
       </c>
       <c r="G14" s="3">
-        <f>G16*1000/(365*24*(49/52))</f>
+        <f t="shared" ref="G14:H14" si="8">G16*1000/(365*24*(49/52))</f>
+        <v>4.7246295778585408</v>
+      </c>
+      <c r="H14" s="3">
+        <f t="shared" si="8"/>
+        <v>4.7246295778585408</v>
+      </c>
+      <c r="I14" s="3">
+        <f>I16*1000/(365*24*(49/52))</f>
         <v>3.6343304445065696</v>
       </c>
-      <c r="H14" s="3">
-        <f t="shared" ref="H14:I14" si="3">H16*1000/(365*24*(49/52))</f>
+      <c r="J14" s="3">
+        <f t="shared" ref="J14:K14" si="9">J16*1000/(365*24*(49/52))</f>
         <v>3.6343304445065696</v>
       </c>
-      <c r="I14" s="3">
-        <f t="shared" si="3"/>
+      <c r="K14" s="3">
+        <f t="shared" si="9"/>
         <v>3.1497530519056935</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1544,16 +1854,22 @@
         <v>1</v>
       </c>
       <c r="G15">
+        <v>1.35</v>
+      </c>
+      <c r="H15">
+        <v>1.35</v>
+      </c>
+      <c r="I15">
         <v>1.0900000000000001</v>
       </c>
-      <c r="H15">
+      <c r="J15">
         <v>0.96</v>
       </c>
-      <c r="I15">
+      <c r="K15">
         <v>0.87</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1570,16 +1886,22 @@
         <v>2</v>
       </c>
       <c r="G16">
+        <v>39</v>
+      </c>
+      <c r="H16">
+        <v>39</v>
+      </c>
+      <c r="I16">
         <v>30</v>
       </c>
-      <c r="H16">
+      <c r="J16">
         <v>30</v>
       </c>
-      <c r="I16">
+      <c r="K16">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>12</v>
       </c>
@@ -1604,8 +1926,14 @@
       <c r="I17" s="3">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J17" s="3">
+        <v>30</v>
+      </c>
+      <c r="K17" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>12</v>
       </c>
@@ -1636,8 +1964,16 @@
         <f>0.1/5.53</f>
         <v>1.8083182640144666E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J18" s="3">
+        <f>0.1/5.53</f>
+        <v>1.8083182640144666E-2</v>
+      </c>
+      <c r="K18" s="3">
+        <f>0.1/5.53</f>
+        <v>1.8083182640144666E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>12</v>
       </c>
@@ -1657,19 +1993,27 @@
         <v>34</v>
       </c>
       <c r="G19" s="3">
+        <f t="shared" ref="G19:H19" si="10">6.4/5.53</f>
+        <v>1.1573236889692586</v>
+      </c>
+      <c r="H19" s="3">
+        <f t="shared" si="10"/>
+        <v>1.1573236889692586</v>
+      </c>
+      <c r="I19" s="3">
         <f>6.4/5.53</f>
         <v>1.1573236889692586</v>
       </c>
-      <c r="H19" s="3">
-        <f t="shared" ref="H19:I19" si="4">6.4/5.53</f>
+      <c r="J19" s="3">
+        <f t="shared" ref="J19:K19" si="11">6.4/5.53</f>
         <v>1.1573236889692586</v>
       </c>
-      <c r="I19" s="3">
-        <f t="shared" si="4"/>
+      <c r="K19" s="3">
+        <f t="shared" si="11"/>
         <v>1.1573236889692586</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>12</v>
       </c>
@@ -1689,19 +2033,27 @@
         <v>34</v>
       </c>
       <c r="G20" s="3">
+        <f t="shared" ref="G20:H20" si="12">1.4/5.53</f>
+        <v>0.25316455696202528</v>
+      </c>
+      <c r="H20" s="3">
+        <f t="shared" si="12"/>
+        <v>0.25316455696202528</v>
+      </c>
+      <c r="I20" s="3">
         <f>1.4/5.53</f>
         <v>0.25316455696202528</v>
       </c>
-      <c r="H20" s="3">
-        <f t="shared" ref="H20:I20" si="5">1.4/5.53</f>
+      <c r="J20" s="3">
+        <f t="shared" ref="J20:K20" si="13">1.4/5.53</f>
         <v>0.25316455696202528</v>
       </c>
-      <c r="I20" s="3">
-        <f t="shared" si="5"/>
+      <c r="K20" s="3">
+        <f t="shared" si="13"/>
         <v>0.25316455696202528</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>12</v>
       </c>
@@ -1726,8 +2078,14 @@
       <c r="I21" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J21" s="3">
+        <v>0</v>
+      </c>
+      <c r="K21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>12</v>
       </c>
@@ -1752,8 +2110,14 @@
       <c r="I22" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J22" s="3">
+        <v>0</v>
+      </c>
+      <c r="K22" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>12</v>
       </c>
@@ -1770,19 +2134,27 @@
         <v>16</v>
       </c>
       <c r="G24" s="3">
-        <f>G25</f>
+        <f t="shared" ref="G24:H24" si="14">G25</f>
         <v>7.3145990404386581</v>
       </c>
       <c r="H24" s="3">
-        <f t="shared" ref="H24:I24" si="6">H25</f>
+        <f t="shared" si="14"/>
         <v>7.3145990404386581</v>
       </c>
       <c r="I24" s="3">
-        <f t="shared" si="6"/>
+        <f>I25</f>
         <v>7.3145990404386581</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J24" s="3">
+        <f t="shared" ref="J24:K24" si="15">J25</f>
+        <v>7.3145990404386581</v>
+      </c>
+      <c r="K24" s="3">
+        <f t="shared" si="15"/>
+        <v>7.3145990404386581</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -1799,19 +2171,27 @@
         <v>20</v>
       </c>
       <c r="G25">
-        <f>G26/$I$40</f>
+        <f>G26/$J$40</f>
         <v>7.3145990404386581</v>
       </c>
       <c r="H25">
-        <f t="shared" ref="H25:I25" si="7">H26/$I$40</f>
+        <f t="shared" ref="H25" si="16">H26/$J$40</f>
         <v>7.3145990404386581</v>
       </c>
       <c r="I25">
-        <f t="shared" si="7"/>
+        <f>I26/$J$40</f>
         <v>7.3145990404386581</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J25">
+        <f t="shared" ref="J25:K25" si="17">J26/$J$40</f>
+        <v>7.3145990404386581</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="17"/>
+        <v>7.3145990404386581</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -1828,19 +2208,27 @@
         <v>21</v>
       </c>
       <c r="G26">
-        <f>G27/$I$37</f>
+        <f>G27/$J$37</f>
         <v>3.2016000000000004</v>
       </c>
       <c r="H26">
-        <f t="shared" ref="H26:I26" si="8">H27/$I$37</f>
+        <f t="shared" ref="H26" si="18">H27/$J$37</f>
         <v>3.2016000000000004</v>
       </c>
       <c r="I26">
-        <f t="shared" si="8"/>
+        <f>I27/$J$37</f>
         <v>3.2016000000000004</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J26">
+        <f t="shared" ref="J26:K26" si="19">J27/$J$37</f>
+        <v>3.2016000000000004</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="19"/>
+        <v>3.2016000000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -1865,8 +2253,14 @@
       <c r="I27">
         <v>6.9</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J27">
+        <v>6.9</v>
+      </c>
+      <c r="K27">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>12</v>
       </c>
@@ -1883,19 +2277,27 @@
         <v>36</v>
       </c>
       <c r="G28" s="3">
-        <f>G30/$I$39</f>
+        <f>G30/$J$39</f>
         <v>0.3652392947103274</v>
       </c>
       <c r="H28" s="3">
-        <f t="shared" ref="H28:I28" si="9">H30/$I$39</f>
+        <f t="shared" ref="H28:H29" si="20">H30/$J$39</f>
         <v>0.3652392947103274</v>
       </c>
       <c r="I28" s="3">
-        <f t="shared" si="9"/>
+        <f>I30/$J$39</f>
         <v>0.3652392947103274</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J28" s="3">
+        <f t="shared" ref="J28:K28" si="21">J30/$J$39</f>
+        <v>0.3652392947103274</v>
+      </c>
+      <c r="K28" s="3">
+        <f t="shared" si="21"/>
+        <v>0.3652392947103274</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>12</v>
       </c>
@@ -1912,19 +2314,27 @@
         <v>36</v>
       </c>
       <c r="G29" s="3">
-        <f>G31/$I$39</f>
+        <f>G31/$J$39</f>
         <v>0.57934508816120911</v>
       </c>
       <c r="H29" s="3">
-        <f t="shared" ref="H29:I29" si="10">H31/$I$39</f>
+        <f t="shared" si="20"/>
         <v>0.57934508816120911</v>
       </c>
       <c r="I29" s="3">
-        <f t="shared" si="10"/>
+        <f>I31/$J$39</f>
         <v>0.57934508816120911</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J29" s="3">
+        <f>J31/$J$39</f>
+        <v>0.57934508816120911</v>
+      </c>
+      <c r="K29" s="3">
+        <f t="shared" ref="K29" si="22">K31/$J$39</f>
+        <v>0.57934508816120911</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -1949,8 +2359,14 @@
       <c r="I30">
         <v>4.3499999999999996</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J30">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="K30">
+        <v>4.3499999999999996</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -1975,71 +2391,116 @@
       <c r="I31">
         <v>6.9</v>
       </c>
-    </row>
-    <row r="36" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="G36" t="s">
+      <c r="J31">
+        <v>6.9</v>
+      </c>
+      <c r="K31">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H36" t="s">
         <v>24</v>
       </c>
-      <c r="H36" s="2" t="s">
+      <c r="I36" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I36">
+      <c r="J36">
         <f>1/1.038</f>
         <v>0.96339113680154143</v>
       </c>
-      <c r="J36" t="s">
+      <c r="K36" t="s">
         <v>27</v>
       </c>
-      <c r="K36" t="s">
+      <c r="L36" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="G37" t="s">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H37" t="s">
         <v>24</v>
       </c>
-      <c r="H37" s="2" t="s">
+      <c r="I37" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I37">
+      <c r="J37">
         <f>1/0.464</f>
         <v>2.1551724137931032</v>
       </c>
-      <c r="J37" t="s">
+      <c r="K37" t="s">
         <v>26</v>
       </c>
-      <c r="K37" t="s">
+      <c r="L37" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="H39" t="s">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I39" t="s">
         <v>19</v>
       </c>
-      <c r="I39">
+      <c r="J39">
         <v>11.91</v>
       </c>
     </row>
-    <row r="40" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="H40" t="s">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>63</v>
+      </c>
+      <c r="I40" t="s">
         <v>23</v>
       </c>
-      <c r="I40">
+      <c r="J40">
         <v>0.43769999999999998</v>
       </c>
-      <c r="J40" t="s">
+      <c r="K40" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="H41" t="s">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>15</v>
+      </c>
+      <c r="B41" t="s">
+        <v>64</v>
+      </c>
+      <c r="I41" t="s">
         <v>39</v>
       </c>
-      <c r="I41">
+      <c r="J41">
         <v>12.36</v>
       </c>
     </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B42">
+        <f>A41*1000000/277777.78</f>
+        <v>53.999999568</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>15</v>
+      </c>
+      <c r="B43" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B44">
+        <f>A43*1000000/(365*52*24)</f>
+        <v>32.929399367755529</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>15</v>
+      </c>
+      <c r="B45" t="s">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Additions to technology catalogue: added CO2 capture of 0 for JRC-IDEES data, Corrected CCS CAPEX for AIDRES 2.0, added ethane cracker technologies and cleaned up accompanying text in the technology_catalogue QMD and HTML files
</commit_message>
<xml_diff>
--- a/input_data/extra_data/extra_data_processes.xlsx
+++ b/input_data/extra_data/extra_data_processes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vitoresearch-my.sharepoint.com/personal/hans_vandeput_vito_be/Documents/Mopo/mopo_repo/input_data/extra_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="334" documentId="8_{EE620E29-61A6-43EA-BFBF-83AA0D58C3C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0504EF02-971D-4BC1-9FD2-EEB7946AD060}"/>
+  <xr:revisionPtr revIDLastSave="335" documentId="8_{EE620E29-61A6-43EA-BFBF-83AA0D58C3C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8280971-2120-4D8E-87A0-010D07E5FE30}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{F2053A1D-A610-4EC9-BADA-756186C5C9C1}"/>
+    <workbookView xWindow="28680" yWindow="-765" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{F2053A1D-A610-4EC9-BADA-756186C5C9C1}"/>
   </bookViews>
   <sheets>
     <sheet name="extra_data" sheetId="1" r:id="rId1"/>
@@ -281,7 +281,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -291,7 +291,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
@@ -658,9 +657,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41472E5A-EAB6-4D4D-BEEA-89BED4F25E24}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
@@ -1344,86 +1343,6 @@
         <v>0.57934508816120911</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1433,8 +1352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3BBEA03-D463-44FB-8E40-6A1CC8E39C5E}">
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView topLeftCell="B12" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28:K29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1532,7 +1451,7 @@
       <c r="L2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="M2" s="9"/>
+      <c r="M2" s="8"/>
     </row>
     <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -1573,13 +1492,13 @@
       <c r="L3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="M3" s="9"/>
+      <c r="M3" s="8"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" t="s">
         <v>45</v>
       </c>
       <c r="D4" t="s">
@@ -1607,10 +1526,10 @@
       <c r="K4">
         <v>0.96</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="L4" t="s">
         <v>50</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="M4" s="7" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1618,7 +1537,7 @@
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" t="s">
         <v>45</v>
       </c>
       <c r="D5" t="s">
@@ -1646,10 +1565,10 @@
       <c r="K5">
         <v>7.87</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" t="s">
         <v>50</v>
       </c>
-      <c r="M5" s="8" t="s">
+      <c r="M5" s="7" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1688,7 +1607,7 @@
       <c r="L6" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="M6" s="9"/>
+      <c r="M6" s="8"/>
     </row>
     <row r="7" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
@@ -1732,7 +1651,7 @@
       <c r="L7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="M7" s="9"/>
+      <c r="M7" s="8"/>
     </row>
     <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
@@ -1762,7 +1681,7 @@
         <v>1.4760989010989012</v>
       </c>
       <c r="I8" s="3">
-        <f t="shared" ref="I8:K8" si="3">0.995/0.7</f>
+        <f t="shared" ref="I8" si="3">0.995/0.7</f>
         <v>1.4214285714285715</v>
       </c>
       <c r="J8" s="3">
@@ -1776,7 +1695,7 @@
       <c r="L8" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="M8" s="9"/>
+      <c r="M8" s="8"/>
     </row>
     <row r="9" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
@@ -1820,7 +1739,7 @@
       <c r="L9" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="M9" s="9"/>
+      <c r="M9" s="8"/>
     </row>
     <row r="10" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
@@ -1857,7 +1776,7 @@
       <c r="L10" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="M10" s="9"/>
+      <c r="M10" s="8"/>
     </row>
     <row r="11" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
@@ -1894,10 +1813,10 @@
       <c r="L11" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="M11" s="9"/>
+      <c r="M11" s="8"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="M12" s="8" t="s">
+      <c r="M12" s="7" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1937,7 +1856,7 @@
         <f t="shared" si="4"/>
         <v>99.31506849315069</v>
       </c>
-      <c r="M13" s="9"/>
+      <c r="M13" s="8"/>
     </row>
     <row r="14" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
@@ -1975,13 +1894,13 @@
         <f t="shared" si="5"/>
         <v>2.9680365296803655</v>
       </c>
-      <c r="M14" s="9"/>
+      <c r="M14" s="8"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" t="s">
         <v>46</v>
       </c>
       <c r="D15" t="s">
@@ -2008,7 +1927,7 @@
       <c r="K15">
         <v>0.87</v>
       </c>
-      <c r="M15" s="8" t="s">
+      <c r="M15" s="7" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2016,7 +1935,7 @@
       <c r="A16" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" t="s">
         <v>46</v>
       </c>
       <c r="D16" t="s">
@@ -2043,7 +1962,7 @@
       <c r="K16">
         <v>26</v>
       </c>
-      <c r="M16" s="8" t="s">
+      <c r="M16" s="7" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2078,7 +1997,7 @@
       <c r="K17" s="3">
         <v>30</v>
       </c>
-      <c r="M17" s="9"/>
+      <c r="M17" s="8"/>
     </row>
     <row r="18" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
@@ -2119,7 +2038,7 @@
         <f t="shared" si="6"/>
         <v>1.8083182640144666E-2</v>
       </c>
-      <c r="M18" s="9"/>
+      <c r="M18" s="8"/>
     </row>
     <row r="19" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
@@ -2160,7 +2079,7 @@
         <f t="shared" si="7"/>
         <v>1.2677262777196154</v>
       </c>
-      <c r="M19" s="9"/>
+      <c r="M19" s="8"/>
     </row>
     <row r="20" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
@@ -2201,7 +2120,7 @@
         <f t="shared" si="8"/>
         <v>0.25316455696202528</v>
       </c>
-      <c r="M20" s="9"/>
+      <c r="M20" s="8"/>
     </row>
     <row r="21" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
@@ -2234,7 +2153,7 @@
       <c r="K21" s="3">
         <v>0</v>
       </c>
-      <c r="M21" s="9"/>
+      <c r="M21" s="8"/>
     </row>
     <row r="22" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
@@ -2267,7 +2186,7 @@
       <c r="K22" s="3">
         <v>0</v>
       </c>
-      <c r="M22" s="9"/>
+      <c r="M22" s="8"/>
     </row>
     <row r="24" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
@@ -2290,7 +2209,7 @@
         <v>7.8849004800000015</v>
       </c>
       <c r="H24" s="3">
-        <f t="shared" ref="G24:H24" si="9">H25</f>
+        <f t="shared" ref="H24" si="9">H25</f>
         <v>7.8849004800000015</v>
       </c>
       <c r="I24" s="3">
@@ -2411,7 +2330,7 @@
       <c r="K27">
         <v>6.9</v>
       </c>
-      <c r="M27" s="8" t="s">
+      <c r="M27" s="7" t="s">
         <v>53</v>
       </c>
     </row>
@@ -2520,7 +2439,7 @@
       <c r="K30">
         <v>4.3499999999999996</v>
       </c>
-      <c r="M30" s="8" t="s">
+      <c r="M30" s="7" t="s">
         <v>53</v>
       </c>
     </row>
@@ -2555,7 +2474,7 @@
       <c r="K31">
         <v>6.9</v>
       </c>
-      <c r="M31" s="8" t="s">
+      <c r="M31" s="7" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>